<commit_message>
R4, R7, R1 mod
</commit_message>
<xml_diff>
--- a/dades/2S1.xlsx
+++ b/dades/2S1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mique_000\Desktop\Jocs (Notes)\Nimby Rails\Transports de Catalunya\Calculadores\dades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E252CF8D-A7BA-47C3-953A-015E854C387E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C87D77-45CD-450C-9513-4F0FBDD7CCA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4103" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4807" uniqueCount="268">
   <si>
     <t>departure</t>
   </si>
@@ -567,6 +567,279 @@
   </si>
   <si>
     <t>R2B.016</t>
+  </si>
+  <si>
+    <t>R8A.001</t>
+  </si>
+  <si>
+    <t>R8A</t>
+  </si>
+  <si>
+    <t>Vilafranca del Penedès</t>
+  </si>
+  <si>
+    <t>R8A.002</t>
+  </si>
+  <si>
+    <t>R8A.003</t>
+  </si>
+  <si>
+    <t>R8A.004</t>
+  </si>
+  <si>
+    <t>R8A.005</t>
+  </si>
+  <si>
+    <t>R8A.006</t>
+  </si>
+  <si>
+    <t>R8A.007</t>
+  </si>
+  <si>
+    <t>R8A.008</t>
+  </si>
+  <si>
+    <t>R8A.009</t>
+  </si>
+  <si>
+    <t>R8A.010</t>
+  </si>
+  <si>
+    <t>R8A.011</t>
+  </si>
+  <si>
+    <t>R8A.012</t>
+  </si>
+  <si>
+    <t>R8A.013</t>
+  </si>
+  <si>
+    <t>R8A.014</t>
+  </si>
+  <si>
+    <t>R8A.015</t>
+  </si>
+  <si>
+    <t>R8A.016</t>
+  </si>
+  <si>
+    <t>R8A.017</t>
+  </si>
+  <si>
+    <t>R8A.018</t>
+  </si>
+  <si>
+    <t>R8A.019</t>
+  </si>
+  <si>
+    <t>R8A.020</t>
+  </si>
+  <si>
+    <t>R8A.021</t>
+  </si>
+  <si>
+    <t>R8A.022</t>
+  </si>
+  <si>
+    <t>R8A.023</t>
+  </si>
+  <si>
+    <t>R8A.024</t>
+  </si>
+  <si>
+    <t>R8A.025</t>
+  </si>
+  <si>
+    <t>R8A.026</t>
+  </si>
+  <si>
+    <t>R8A.027</t>
+  </si>
+  <si>
+    <t>R8A.028</t>
+  </si>
+  <si>
+    <t>R8A.029</t>
+  </si>
+  <si>
+    <t>R8A.030</t>
+  </si>
+  <si>
+    <t>R8A.031</t>
+  </si>
+  <si>
+    <t>R8A.032</t>
+  </si>
+  <si>
+    <t>R8A.033</t>
+  </si>
+  <si>
+    <t>R8A.034</t>
+  </si>
+  <si>
+    <t>R8A.035</t>
+  </si>
+  <si>
+    <t>R8A.036</t>
+  </si>
+  <si>
+    <t>R8A.037</t>
+  </si>
+  <si>
+    <t>R8A.038</t>
+  </si>
+  <si>
+    <t>R8A.039</t>
+  </si>
+  <si>
+    <t>R8A.040</t>
+  </si>
+  <si>
+    <t>R8A.041</t>
+  </si>
+  <si>
+    <t>R8A.042</t>
+  </si>
+  <si>
+    <t>R8A.043</t>
+  </si>
+  <si>
+    <t>R8A.044</t>
+  </si>
+  <si>
+    <t>R8A.045</t>
+  </si>
+  <si>
+    <t>R8A.046</t>
+  </si>
+  <si>
+    <t>R8A.047</t>
+  </si>
+  <si>
+    <t>R8A.048</t>
+  </si>
+  <si>
+    <t>R8A.049</t>
+  </si>
+  <si>
+    <t>R8A.050</t>
+  </si>
+  <si>
+    <t>R8A.051</t>
+  </si>
+  <si>
+    <t>R8A.052</t>
+  </si>
+  <si>
+    <t>R8A.053</t>
+  </si>
+  <si>
+    <t>R8A.054</t>
+  </si>
+  <si>
+    <t>R8A.055</t>
+  </si>
+  <si>
+    <t>R8A.056</t>
+  </si>
+  <si>
+    <t>R8A.057</t>
+  </si>
+  <si>
+    <t>R8A.058</t>
+  </si>
+  <si>
+    <t>R8A.059</t>
+  </si>
+  <si>
+    <t>R8A.060</t>
+  </si>
+  <si>
+    <t>R8A.061</t>
+  </si>
+  <si>
+    <t>R8A.062</t>
+  </si>
+  <si>
+    <t>R8A.063</t>
+  </si>
+  <si>
+    <t>R8A.064</t>
+  </si>
+  <si>
+    <t>R8A.065</t>
+  </si>
+  <si>
+    <t>R8A.066</t>
+  </si>
+  <si>
+    <t>R8A.067</t>
+  </si>
+  <si>
+    <t>R8A.068</t>
+  </si>
+  <si>
+    <t>R8A.069</t>
+  </si>
+  <si>
+    <t>R8A.070</t>
+  </si>
+  <si>
+    <t>R8A.071</t>
+  </si>
+  <si>
+    <t>R8A.072</t>
+  </si>
+  <si>
+    <t>R8B</t>
+  </si>
+  <si>
+    <t>R8B.001</t>
+  </si>
+  <si>
+    <t>R8B.002</t>
+  </si>
+  <si>
+    <t>R8B.003</t>
+  </si>
+  <si>
+    <t>R8B.004</t>
+  </si>
+  <si>
+    <t>R8B.005</t>
+  </si>
+  <si>
+    <t>R8B.006</t>
+  </si>
+  <si>
+    <t>R8B.007</t>
+  </si>
+  <si>
+    <t>R8B.008</t>
+  </si>
+  <si>
+    <t>R8B.009</t>
+  </si>
+  <si>
+    <t>R8B.010</t>
+  </si>
+  <si>
+    <t>R8B.011</t>
+  </si>
+  <si>
+    <t>R8B.012</t>
+  </si>
+  <si>
+    <t>R8B.013</t>
+  </si>
+  <si>
+    <t>R8B.014</t>
+  </si>
+  <si>
+    <t>R8B.015</t>
+  </si>
+  <si>
+    <t>R8B.016</t>
   </si>
 </sst>
 </file>
@@ -617,15 +890,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -636,6 +914,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7511E47-15C1-4278-9418-72B3FF957562}" name="Taula1" displayName="Taula1" ref="A1:E1209" totalsRowShown="0">
+  <autoFilter ref="A1:E1209" xr:uid="{B7511E47-15C1-4278-9418-72B3FF957562}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B8ABD6E3-F25D-4ADA-ABE9-4AED04423A6F}" name="station"/>
+    <tableColumn id="2" xr3:uid="{1FDA469A-5F2A-4595-AAE4-CEF9AF2DBBD1}" name="departure" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{6F0EAADD-87A4-4ED3-8047-24BC263548FA}" name="train_number"/>
+    <tableColumn id="4" xr3:uid="{ABE58276-1D89-4037-88B5-3B17FD7FA4DF}" name="service_code"/>
+    <tableColumn id="5" xr3:uid="{580AE635-0F6F-4F24-8D10-09C921A6CDD6}" name="destination"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -901,18 +1193,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1033"/>
+  <dimension ref="A1:J1209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A992" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B947" sqref="B947:B1033"/>
+    <sheetView tabSelected="1" topLeftCell="A1170" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1182" sqref="B1182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19317,8 +19609,3167 @@
         <v>81</v>
       </c>
     </row>
+    <row r="1034" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1034" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1034" s="1">
+        <v>0.21427083333333333</v>
+      </c>
+      <c r="C1034" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1034" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1034" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1035" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1035" s="1">
+        <v>0.21895833333333334</v>
+      </c>
+      <c r="C1035" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1035" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1035" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1036" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1036" s="1">
+        <v>0.28164351851851849</v>
+      </c>
+      <c r="C1036" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1036" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1036" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1037" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1037" s="1">
+        <v>0.2860300925925926</v>
+      </c>
+      <c r="C1037" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1037" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1037" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1038" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1038" s="1">
+        <f>B1034+(2/24)</f>
+        <v>0.29760416666666667</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1038" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1038" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1039" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1039" s="1">
+        <f t="shared" ref="B1039:B1102" si="17">B1035+(2/24)</f>
+        <v>0.30229166666666668</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1039" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1039" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1040" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1040" s="1">
+        <f t="shared" si="17"/>
+        <v>0.3649768518518518</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1040" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1040" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1041" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1041" s="1">
+        <f t="shared" si="17"/>
+        <v>0.36936342592592591</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1041" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1041" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1042" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1042" s="1">
+        <f t="shared" si="17"/>
+        <v>0.38093749999999998</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1042" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1042" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1043" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1043" s="1">
+        <f t="shared" si="17"/>
+        <v>0.385625</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1043" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1043" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1044" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1044" s="1">
+        <f t="shared" si="17"/>
+        <v>0.44831018518518512</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1044" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1044" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1045" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1045" s="1">
+        <f t="shared" si="17"/>
+        <v>0.45269675925925923</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1045" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1045" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1046" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1046" s="1">
+        <f t="shared" si="17"/>
+        <v>0.4642708333333333</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1046" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1047" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1047" s="1">
+        <f t="shared" si="17"/>
+        <v>0.46895833333333331</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1047" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1048" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1048" s="1">
+        <f t="shared" si="17"/>
+        <v>0.53164351851851843</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1048" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1048" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1049" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1049" s="1">
+        <f t="shared" si="17"/>
+        <v>0.5360300925925926</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1049" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1049" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1050" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1050" s="1">
+        <f t="shared" si="17"/>
+        <v>0.54760416666666667</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1050" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1051" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1051" s="1">
+        <f t="shared" si="17"/>
+        <v>0.55229166666666663</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1051" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1052" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1052" s="1">
+        <f t="shared" si="17"/>
+        <v>0.6149768518518518</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1052" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1052" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1053" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1053" s="1">
+        <f t="shared" si="17"/>
+        <v>0.61936342592592597</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1053" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1054" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1054" s="1">
+        <f t="shared" si="17"/>
+        <v>0.63093750000000004</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1054" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1055" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1055" s="1">
+        <f t="shared" si="17"/>
+        <v>0.635625</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1055" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1056" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1056" s="1">
+        <f t="shared" si="17"/>
+        <v>0.69831018518518517</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1056" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1056" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1057" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1057" s="1">
+        <f t="shared" si="17"/>
+        <v>0.70269675925925934</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1057" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1057" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1058" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1058" s="1">
+        <f t="shared" si="17"/>
+        <v>0.71427083333333341</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1058" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1058" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1059" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1059" s="1">
+        <f t="shared" si="17"/>
+        <v>0.71895833333333337</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1060" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1060" s="1">
+        <f t="shared" si="17"/>
+        <v>0.78164351851851854</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1060" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1060" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1061" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1061" s="1">
+        <f t="shared" si="17"/>
+        <v>0.78603009259259271</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1061" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1061" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1062" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1062" s="1">
+        <f t="shared" si="17"/>
+        <v>0.79760416666666678</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1062" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1063" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1063" s="1">
+        <f t="shared" si="17"/>
+        <v>0.80229166666666674</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1063" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1064" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1064" s="1">
+        <f t="shared" si="17"/>
+        <v>0.86497685185185191</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1064" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1064" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1065" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1065" s="1">
+        <f t="shared" si="17"/>
+        <v>0.86936342592592608</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1065" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1066" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1066" s="1">
+        <f t="shared" si="17"/>
+        <v>0.88093750000000015</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1066" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1067" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1067" s="1">
+        <f t="shared" si="17"/>
+        <v>0.88562500000000011</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1067" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1068" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1068" s="1">
+        <f t="shared" si="17"/>
+        <v>0.94831018518518528</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1068" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1068" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1069" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1069" s="1">
+        <f t="shared" si="17"/>
+        <v>0.95269675925925945</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1069" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1070" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1070" s="1">
+        <v>0.23997685185185183</v>
+      </c>
+      <c r="C1070" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1070" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1071" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1071" s="1">
+        <v>0.24436342592592594</v>
+      </c>
+      <c r="C1071" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1071" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1072" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1072" s="1">
+        <v>0.25593749999999998</v>
+      </c>
+      <c r="C1072" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1072" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1072" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1073" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1073" s="1">
+        <v>0.260625</v>
+      </c>
+      <c r="C1073" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1073" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1073" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1074" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1074" s="1">
+        <f t="shared" si="17"/>
+        <v>0.32331018518518517</v>
+      </c>
+      <c r="C1074" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1074" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1074" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1075" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1075" s="1">
+        <f t="shared" si="17"/>
+        <v>0.32769675925925928</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1075" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1075" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1076" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1076" s="1">
+        <f t="shared" si="17"/>
+        <v>0.3392708333333333</v>
+      </c>
+      <c r="C1076" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1076" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1076" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1077" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1077" s="1">
+        <f t="shared" si="17"/>
+        <v>0.34395833333333331</v>
+      </c>
+      <c r="C1077" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1077" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1077" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1078" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1078" s="1">
+        <f t="shared" si="17"/>
+        <v>0.40664351851851849</v>
+      </c>
+      <c r="C1078" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1078" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1079" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1079" s="1">
+        <f t="shared" si="17"/>
+        <v>0.4110300925925926</v>
+      </c>
+      <c r="C1079" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1079" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1079" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1080" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1080" s="1">
+        <f t="shared" si="17"/>
+        <v>0.42260416666666661</v>
+      </c>
+      <c r="C1080" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1080" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1080" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1081" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1081" s="1">
+        <f t="shared" si="17"/>
+        <v>0.42729166666666663</v>
+      </c>
+      <c r="C1081" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1081" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1081" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1082" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1082" s="1">
+        <f t="shared" si="17"/>
+        <v>0.4899768518518518</v>
+      </c>
+      <c r="C1082" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1082" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1083" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1083" s="1">
+        <f t="shared" si="17"/>
+        <v>0.49436342592592591</v>
+      </c>
+      <c r="C1083" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1083" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1084" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1084" s="1">
+        <f t="shared" si="17"/>
+        <v>0.50593749999999993</v>
+      </c>
+      <c r="C1084" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1084" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1084" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1085" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1085" s="1">
+        <f t="shared" si="17"/>
+        <v>0.510625</v>
+      </c>
+      <c r="C1085" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1085" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1085" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1086" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1086" s="1">
+        <f t="shared" si="17"/>
+        <v>0.57331018518518517</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1086" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1087" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1087" s="1">
+        <f t="shared" si="17"/>
+        <v>0.57769675925925923</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1087" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1087" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1088" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1088" s="1">
+        <f t="shared" si="17"/>
+        <v>0.5892708333333333</v>
+      </c>
+      <c r="C1088" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1088" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1088" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1089" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1089" s="1">
+        <f t="shared" si="17"/>
+        <v>0.59395833333333337</v>
+      </c>
+      <c r="C1089" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1089" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1089" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1090" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1090" s="1">
+        <f t="shared" si="17"/>
+        <v>0.65664351851851854</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1090" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1091" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1091" s="1">
+        <f t="shared" si="17"/>
+        <v>0.6610300925925926</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1091" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1091" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1092" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1092" s="1">
+        <f t="shared" si="17"/>
+        <v>0.67260416666666667</v>
+      </c>
+      <c r="C1092" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1092" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1092" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1093" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1093" s="1">
+        <f t="shared" si="17"/>
+        <v>0.67729166666666674</v>
+      </c>
+      <c r="C1093" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1093" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1093" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1094" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1094" s="1">
+        <f t="shared" si="17"/>
+        <v>0.73997685185185191</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1094" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1094" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1095" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1095" s="1">
+        <f t="shared" si="17"/>
+        <v>0.74436342592592597</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1095" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1096" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1096" s="1">
+        <f t="shared" si="17"/>
+        <v>0.75593750000000004</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1096" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1097" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1097" s="1">
+        <f t="shared" si="17"/>
+        <v>0.76062500000000011</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1097" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1097" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1098" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1098" s="1">
+        <f t="shared" si="17"/>
+        <v>0.82331018518518528</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1098" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1098" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1099" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1099" s="1">
+        <f t="shared" si="17"/>
+        <v>0.82769675925925934</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1099" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1100" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1100" s="1">
+        <f t="shared" si="17"/>
+        <v>0.83927083333333341</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1100" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1101" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1101" s="1">
+        <f t="shared" si="17"/>
+        <v>0.84395833333333348</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1101" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1101" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1102" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1102" s="1">
+        <f t="shared" si="17"/>
+        <v>0.90664351851851865</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1102" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1103" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1103" s="1">
+        <f t="shared" ref="B1103:B1105" si="18">B1099+(2/24)</f>
+        <v>0.91103009259259271</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1103" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1104" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1104" s="1">
+        <f t="shared" si="18"/>
+        <v>0.92260416666666678</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1104" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1104" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1105" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1105" s="1">
+        <f t="shared" si="18"/>
+        <v>0.92729166666666685</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1105" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1105" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1106" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1106" s="1">
+        <f>B1034+(0.5/24)</f>
+        <v>0.23510416666666667</v>
+      </c>
+      <c r="C1106" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1106" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1107" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1107" s="1">
+        <f t="shared" ref="B1107:B1134" si="19">B1035+(0.5/24)</f>
+        <v>0.23979166666666668</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1107" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1108" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1108" s="1">
+        <f t="shared" si="19"/>
+        <v>0.3024768518518518</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1108" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1108" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1109" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1109" s="1">
+        <f t="shared" si="19"/>
+        <v>0.30686342592592591</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1109" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1109" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1110" s="1">
+        <f t="shared" si="19"/>
+        <v>0.31843749999999998</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1110" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1111" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1111" s="1">
+        <f t="shared" si="19"/>
+        <v>0.323125</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1111" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1111" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1112" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1112" s="1">
+        <f t="shared" si="19"/>
+        <v>0.38581018518518512</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1112" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1113" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1113" s="1">
+        <f t="shared" si="19"/>
+        <v>0.39019675925925923</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1113" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1114" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1114" s="1">
+        <f t="shared" si="19"/>
+        <v>0.4017708333333333</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1114" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1115" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1115" s="1">
+        <f t="shared" si="19"/>
+        <v>0.40645833333333331</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1115" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1115" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1116" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1116" s="1">
+        <f t="shared" si="19"/>
+        <v>0.46914351851851843</v>
+      </c>
+      <c r="C1116" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1116" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1117" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1117" s="1">
+        <f t="shared" si="19"/>
+        <v>0.47353009259259254</v>
+      </c>
+      <c r="C1117" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1117" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1117" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1118" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1118" s="1">
+        <f t="shared" si="19"/>
+        <v>0.48510416666666661</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1118" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1119" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1119" s="1">
+        <f t="shared" si="19"/>
+        <v>0.48979166666666663</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1119" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1119" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1120" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1120" s="1">
+        <f t="shared" si="19"/>
+        <v>0.5524768518518518</v>
+      </c>
+      <c r="C1120" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1120" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1120" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1121" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1121" s="1">
+        <f t="shared" si="19"/>
+        <v>0.55686342592592597</v>
+      </c>
+      <c r="C1121" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1121" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1122" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1122" s="1">
+        <f t="shared" si="19"/>
+        <v>0.56843750000000004</v>
+      </c>
+      <c r="C1122" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1122" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1122" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1123" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1123" s="1">
+        <f t="shared" si="19"/>
+        <v>0.573125</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1123" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1123" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1124" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1124" s="1">
+        <f t="shared" si="19"/>
+        <v>0.63581018518518517</v>
+      </c>
+      <c r="C1124" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1124" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1125" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1125" s="1">
+        <f t="shared" si="19"/>
+        <v>0.64019675925925934</v>
+      </c>
+      <c r="C1125" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1125" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1125" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1126" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1126" s="1">
+        <f t="shared" si="19"/>
+        <v>0.65177083333333341</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1126" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1126" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1127" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1127" s="1">
+        <f t="shared" si="19"/>
+        <v>0.65645833333333337</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1127" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1127" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1128" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1128" s="1">
+        <f t="shared" si="19"/>
+        <v>0.71914351851851854</v>
+      </c>
+      <c r="C1128" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1128" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1128" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1129" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1129" s="1">
+        <f t="shared" si="19"/>
+        <v>0.72353009259259271</v>
+      </c>
+      <c r="C1129" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1129" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1130" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1130" s="1">
+        <f t="shared" si="19"/>
+        <v>0.73510416666666678</v>
+      </c>
+      <c r="C1130" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1130" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1130" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1131" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1131" s="1">
+        <f t="shared" si="19"/>
+        <v>0.73979166666666674</v>
+      </c>
+      <c r="C1131" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1131" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1131" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1132" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1132" s="1">
+        <f t="shared" si="19"/>
+        <v>0.80247685185185191</v>
+      </c>
+      <c r="C1132" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1132" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1132" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1133" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1133" s="1">
+        <f t="shared" si="19"/>
+        <v>0.80686342592592608</v>
+      </c>
+      <c r="C1133" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1133" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1133" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1134" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1134" s="1">
+        <f t="shared" si="19"/>
+        <v>0.81843750000000015</v>
+      </c>
+      <c r="C1134" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1134" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1134" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1135" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1135" s="1">
+        <f t="shared" ref="B1135:B1170" si="20">B1063+(0.5/24)</f>
+        <v>0.82312500000000011</v>
+      </c>
+      <c r="C1135" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1135" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1135" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1136" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1136" s="1">
+        <f t="shared" si="20"/>
+        <v>0.88581018518518528</v>
+      </c>
+      <c r="C1136" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1136" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1137" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1137" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89019675925925945</v>
+      </c>
+      <c r="C1137" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1137" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1137" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1138" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1138" s="1">
+        <f t="shared" si="20"/>
+        <v>0.90177083333333352</v>
+      </c>
+      <c r="C1138" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1138" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1138" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1139" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1139" s="1">
+        <f t="shared" si="20"/>
+        <v>0.90645833333333348</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1139" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1139" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1140" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1140" s="1">
+        <f t="shared" si="20"/>
+        <v>0.96914351851851865</v>
+      </c>
+      <c r="C1140" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1140" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1141" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1141" s="1">
+        <f t="shared" si="20"/>
+        <v>0.97353009259259282</v>
+      </c>
+      <c r="C1141" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1141" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1141" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1142" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1142" s="1">
+        <f t="shared" si="20"/>
+        <v>0.26081018518518517</v>
+      </c>
+      <c r="C1142" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1142" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1142" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1143" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1143" s="1">
+        <f t="shared" si="20"/>
+        <v>0.26519675925925928</v>
+      </c>
+      <c r="C1143" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1143" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1143" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1144" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1144" s="1">
+        <f t="shared" si="20"/>
+        <v>0.2767708333333333</v>
+      </c>
+      <c r="C1144" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1144" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1144" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1145" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1145" s="1">
+        <f t="shared" si="20"/>
+        <v>0.28145833333333331</v>
+      </c>
+      <c r="C1145" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1145" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1145" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1146" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1146" s="1">
+        <f t="shared" si="20"/>
+        <v>0.34414351851851849</v>
+      </c>
+      <c r="C1146" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1146" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1147" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1147" s="1">
+        <f t="shared" si="20"/>
+        <v>0.3485300925925926</v>
+      </c>
+      <c r="C1147" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1147" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1147" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1148" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1148" s="1">
+        <f t="shared" si="20"/>
+        <v>0.36010416666666661</v>
+      </c>
+      <c r="C1148" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1148" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1148" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1149" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1149" s="1">
+        <f t="shared" si="20"/>
+        <v>0.36479166666666663</v>
+      </c>
+      <c r="C1149" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1149" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1149" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1150" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1150" s="1">
+        <f t="shared" si="20"/>
+        <v>0.4274768518518518</v>
+      </c>
+      <c r="C1150" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1150" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1150" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1151" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1151" s="1">
+        <f t="shared" si="20"/>
+        <v>0.43186342592592591</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1151" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1151" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1152" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1152" s="1">
+        <f t="shared" si="20"/>
+        <v>0.44343749999999993</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1152" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1152" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1153" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1153" s="1">
+        <f t="shared" si="20"/>
+        <v>0.44812499999999994</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1153" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1153" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1154" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1154" s="1">
+        <f t="shared" si="20"/>
+        <v>0.51081018518518517</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1154" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1155" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1155" s="1">
+        <f t="shared" si="20"/>
+        <v>0.51519675925925923</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1155" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1155" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1156" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1156" s="1">
+        <f t="shared" si="20"/>
+        <v>0.5267708333333333</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1156" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1156" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1157" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1157" s="1">
+        <f t="shared" si="20"/>
+        <v>0.53145833333333337</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1157" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1157" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1158" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1158" s="1">
+        <f t="shared" si="20"/>
+        <v>0.59414351851851854</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1158" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1158" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1159" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1159" s="1">
+        <f t="shared" si="20"/>
+        <v>0.5985300925925926</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1159" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1159" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1160" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1160" s="1">
+        <f t="shared" si="20"/>
+        <v>0.61010416666666667</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1160" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1160" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1161" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1161" s="1">
+        <f t="shared" si="20"/>
+        <v>0.61479166666666674</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1161" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1161" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1162" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1162" s="1">
+        <f t="shared" si="20"/>
+        <v>0.67747685185185191</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1162" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1162" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1163" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1163" s="1">
+        <f t="shared" si="20"/>
+        <v>0.68186342592592597</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1163" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1163" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1164" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1164" s="1">
+        <f t="shared" si="20"/>
+        <v>0.69343750000000004</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1164" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1164" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1165" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1165" s="1">
+        <f t="shared" si="20"/>
+        <v>0.69812500000000011</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1165" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1165" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1166" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1166" s="1">
+        <f t="shared" si="20"/>
+        <v>0.76081018518518528</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1166" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1166" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1167" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1167" s="1">
+        <f t="shared" si="20"/>
+        <v>0.76519675925925934</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1167" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1168" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1168" s="1">
+        <f t="shared" si="20"/>
+        <v>0.77677083333333341</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1168" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1168" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1169" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1169" s="1">
+        <f t="shared" si="20"/>
+        <v>0.78145833333333348</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1169" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1170" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1170" s="1">
+        <f t="shared" si="20"/>
+        <v>0.84414351851851865</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1170" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1171" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1171" s="1">
+        <f t="shared" ref="B1171:B1177" si="21">B1099+(0.5/24)</f>
+        <v>0.84853009259259271</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1171" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1172" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1172" s="1">
+        <f t="shared" si="21"/>
+        <v>0.86010416666666678</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1172" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1172" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1173" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1173" s="1">
+        <f t="shared" si="21"/>
+        <v>0.86479166666666685</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1173" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1173" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1174" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1174" s="1">
+        <f t="shared" si="21"/>
+        <v>0.92747685185185202</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1174" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1174" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1175" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1175" s="1">
+        <f t="shared" si="21"/>
+        <v>0.93186342592592608</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1175" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1175" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1176" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1176" s="1">
+        <f t="shared" si="21"/>
+        <v>0.94343750000000015</v>
+      </c>
+      <c r="C1176" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1176" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1176" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1177" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1177" s="1">
+        <f t="shared" si="21"/>
+        <v>0.94812500000000022</v>
+      </c>
+      <c r="C1177" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1177" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1177" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1178" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1178" s="1">
+        <v>0.29206018518518517</v>
+      </c>
+      <c r="C1178" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1178" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1178" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1179" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1179" s="1">
+        <v>0.29644675925925928</v>
+      </c>
+      <c r="C1179" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1179" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1179" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1180" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1180" s="1">
+        <v>0.30802083333333335</v>
+      </c>
+      <c r="C1180" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1180" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1180" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1181" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1181" s="1">
+        <v>0.31270833333333331</v>
+      </c>
+      <c r="C1181" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1181" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1181" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1182" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1182" s="1">
+        <f>B1178+(2/24)</f>
+        <v>0.37539351851851849</v>
+      </c>
+      <c r="C1182" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1182" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1182" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1183" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1183" s="1">
+        <f t="shared" ref="B1183:B1209" si="22">B1179+(2/24)</f>
+        <v>0.3797800925925926</v>
+      </c>
+      <c r="C1183" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1183" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1183" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1184" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1184" s="1">
+        <f t="shared" si="22"/>
+        <v>0.39135416666666667</v>
+      </c>
+      <c r="C1184" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1184" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1184" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1185" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1185" s="1">
+        <f t="shared" si="22"/>
+        <v>0.39604166666666663</v>
+      </c>
+      <c r="C1185" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1185" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1185" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1186" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1186" s="1">
+        <f t="shared" si="22"/>
+        <v>0.4587268518518518</v>
+      </c>
+      <c r="C1186" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1186" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1186" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1187" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1187" s="1">
+        <f t="shared" si="22"/>
+        <v>0.46311342592592591</v>
+      </c>
+      <c r="C1187" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1187" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1187" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1188" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1188" s="1">
+        <f t="shared" si="22"/>
+        <v>0.47468749999999998</v>
+      </c>
+      <c r="C1188" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1188" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1188" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1189" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1189" s="1">
+        <f t="shared" si="22"/>
+        <v>0.47937499999999994</v>
+      </c>
+      <c r="C1189" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1189" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1189" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1190" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1190" s="1">
+        <f t="shared" si="22"/>
+        <v>0.54206018518518517</v>
+      </c>
+      <c r="C1190" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1190" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1190" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1191" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1191" s="1">
+        <f t="shared" si="22"/>
+        <v>0.54644675925925923</v>
+      </c>
+      <c r="C1191" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1191" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1191" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1192" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1192" s="1">
+        <f t="shared" si="22"/>
+        <v>0.5580208333333333</v>
+      </c>
+      <c r="C1192" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1192" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1192" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1193" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1193" s="1">
+        <f t="shared" si="22"/>
+        <v>0.56270833333333325</v>
+      </c>
+      <c r="C1193" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1193" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1193" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1194" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1194" s="1">
+        <f t="shared" si="22"/>
+        <v>0.62539351851851854</v>
+      </c>
+      <c r="C1194" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1194" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1194" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1195" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1195" s="1">
+        <f t="shared" si="22"/>
+        <v>0.6297800925925926</v>
+      </c>
+      <c r="C1195" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1195" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1195" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1196" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1196" s="1">
+        <f t="shared" si="22"/>
+        <v>0.64135416666666667</v>
+      </c>
+      <c r="C1196" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1196" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1196" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1197" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1197" s="1">
+        <f t="shared" si="22"/>
+        <v>0.64604166666666663</v>
+      </c>
+      <c r="C1197" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1197" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1197" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1198" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1198" s="1">
+        <f t="shared" si="22"/>
+        <v>0.70872685185185191</v>
+      </c>
+      <c r="C1198" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1198" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1198" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1199" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1199" s="1">
+        <f t="shared" si="22"/>
+        <v>0.71311342592592597</v>
+      </c>
+      <c r="C1199" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1199" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1199" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1200" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1200" s="1">
+        <f t="shared" si="22"/>
+        <v>0.72468750000000004</v>
+      </c>
+      <c r="C1200" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1200" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1200" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1201" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1201" s="1">
+        <f t="shared" si="22"/>
+        <v>0.729375</v>
+      </c>
+      <c r="C1201" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1201" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1201" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1202" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1202" s="1">
+        <f t="shared" si="22"/>
+        <v>0.79206018518518528</v>
+      </c>
+      <c r="C1202" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1202" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1202" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1203" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1203" s="1">
+        <f t="shared" si="22"/>
+        <v>0.79644675925925934</v>
+      </c>
+      <c r="C1203" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1203" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1203" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1204" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1204" s="1">
+        <f t="shared" si="22"/>
+        <v>0.80802083333333341</v>
+      </c>
+      <c r="C1204" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1204" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1204" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1205" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1205" s="1">
+        <f t="shared" si="22"/>
+        <v>0.81270833333333337</v>
+      </c>
+      <c r="C1205" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1205" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1205" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1206" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1206" s="1">
+        <f t="shared" si="22"/>
+        <v>0.87539351851851865</v>
+      </c>
+      <c r="C1206" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1206" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1206" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1207" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1207" s="1">
+        <f t="shared" si="22"/>
+        <v>0.87978009259259271</v>
+      </c>
+      <c r="C1207" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1207" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1207" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1208" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1208" s="1">
+        <f t="shared" si="22"/>
+        <v>0.89135416666666678</v>
+      </c>
+      <c r="C1208" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1208" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1208" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1209" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1209" s="1">
+        <f t="shared" si="22"/>
+        <v>0.89604166666666674</v>
+      </c>
+      <c r="C1209" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1209" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1209" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>